<commit_message>
added to regression analysis script
</commit_message>
<xml_diff>
--- a/R_scripts/predictor_variables.xlsx
+++ b/R_scripts/predictor_variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kayle\Documents\Quercus_IUCN_samp_sims\R_scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9C67E146-C2EE-432F-8E4A-D162C1F5C5F0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57204C2C-3DE7-4CF9-8FF0-79C20071727F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4EB2B3E0-7A11-4E9C-9E5A-6DDEDA922F00}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>QUAC</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>Column1</t>
+  </si>
+  <si>
+    <t>Prop. Alleles captured in n=50</t>
   </si>
 </sst>
 </file>
@@ -174,8 +177,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E284B342-EC32-464F-B7EB-28AF6260B4F3}" name="Table1" displayName="Table1" ref="A1:O5" totalsRowShown="0">
-  <autoFilter ref="A1:O5" xr:uid="{12C84DC8-89C1-43B3-AED6-4A576F9E3840}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E284B342-EC32-464F-B7EB-28AF6260B4F3}" name="Table1" displayName="Table1" ref="A1:O6" totalsRowShown="0">
+  <autoFilter ref="A1:O6" xr:uid="{12C84DC8-89C1-43B3-AED6-4A576F9E3840}"/>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{71897B3A-2B4C-4967-8EC8-49121365912E}" name="Column1" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{2F409399-66E5-4DC1-9685-DBB948CE7266}" name="QUAC"/>
@@ -494,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D82BC7BF-D731-4646-A03F-549F50F3F39A}">
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:O5"/>
+      <selection sqref="A1:O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,142 +604,189 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B3">
-        <v>0.13</v>
+        <v>0.876</v>
       </c>
       <c r="C3">
-        <v>0.14199999999999999</v>
+        <v>0.84399999999999997</v>
       </c>
       <c r="D3">
-        <v>0.19500000000000001</v>
+        <v>0.88900000000000001</v>
       </c>
       <c r="E3">
-        <v>0.06</v>
+        <v>0.84399999999999997</v>
       </c>
       <c r="F3">
-        <v>4.3999999999999997E-2</v>
+        <v>0.92300000000000004</v>
       </c>
       <c r="G3">
-        <v>7.3999999999999996E-2</v>
+        <v>0.91400000000000003</v>
       </c>
       <c r="H3">
-        <v>7.6999999999999999E-2</v>
+        <v>0.86</v>
       </c>
       <c r="I3">
-        <v>0.185</v>
+        <v>0.89200000000000002</v>
       </c>
       <c r="J3">
-        <v>0.14000000000000001</v>
+        <v>0.89500000000000002</v>
       </c>
       <c r="K3">
-        <v>5.8999999999999997E-2</v>
+        <v>0.89300000000000002</v>
       </c>
       <c r="L3">
-        <v>0.14499999999999999</v>
+        <v>0.90100000000000002</v>
       </c>
       <c r="M3">
-        <v>0.16400000000000001</v>
+        <v>0.877</v>
       </c>
       <c r="N3">
-        <v>1.2999999999999999E-2</v>
+        <v>0.97799999999999998</v>
       </c>
       <c r="O3">
-        <v>3.1E-2</v>
+        <v>0.95099999999999996</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B4">
-        <v>530</v>
+        <v>0.13</v>
       </c>
       <c r="C4">
-        <v>3460</v>
+        <v>0.14199999999999999</v>
       </c>
       <c r="D4">
-        <v>540</v>
+        <v>0.19500000000000001</v>
       </c>
       <c r="E4">
-        <v>1035</v>
+        <v>0.06</v>
       </c>
       <c r="F4">
-        <v>3000</v>
+        <v>4.3999999999999997E-2</v>
       </c>
       <c r="G4">
-        <v>8400</v>
+        <v>7.3999999999999996E-2</v>
       </c>
       <c r="H4">
-        <v>20000</v>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="I4">
-        <v>500</v>
+        <v>0.185</v>
       </c>
       <c r="J4">
-        <v>325</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="K4">
-        <v>5150</v>
+        <v>5.8999999999999997E-2</v>
       </c>
       <c r="L4">
-        <v>300</v>
+        <v>0.14499999999999999</v>
       </c>
       <c r="M4">
-        <v>1000</v>
+        <v>0.16400000000000001</v>
       </c>
       <c r="N4">
-        <v>13000</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="O4">
-        <v>10500</v>
+        <v>3.1E-2</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>530</v>
+      </c>
+      <c r="C5">
+        <v>3460</v>
+      </c>
+      <c r="D5">
+        <v>540</v>
+      </c>
+      <c r="E5">
+        <v>1035</v>
+      </c>
+      <c r="F5">
+        <v>3000</v>
+      </c>
+      <c r="G5">
+        <v>8400</v>
+      </c>
+      <c r="H5">
+        <v>20000</v>
+      </c>
+      <c r="I5">
+        <v>500</v>
+      </c>
+      <c r="J5">
+        <v>325</v>
+      </c>
+      <c r="K5">
+        <v>5150</v>
+      </c>
+      <c r="L5">
+        <v>300</v>
+      </c>
+      <c r="M5">
+        <v>1000</v>
+      </c>
+      <c r="N5">
+        <v>13000</v>
+      </c>
+      <c r="O5">
+        <v>10500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>4</v>
       </c>
-      <c r="C5">
+      <c r="C6">
         <v>10</v>
       </c>
-      <c r="D5">
+      <c r="D6">
         <v>9</v>
       </c>
-      <c r="E5">
+      <c r="E6">
         <v>8</v>
       </c>
-      <c r="F5">
+      <c r="F6">
         <v>3</v>
       </c>
-      <c r="G5">
+      <c r="G6">
         <v>10</v>
       </c>
-      <c r="H5">
+      <c r="H6">
         <v>4</v>
       </c>
-      <c r="I5">
+      <c r="I6">
         <v>5</v>
       </c>
-      <c r="J5">
+      <c r="J6">
         <v>3</v>
       </c>
-      <c r="K5">
+      <c r="K6">
         <v>19</v>
       </c>
-      <c r="L5">
+      <c r="L6">
         <v>4</v>
       </c>
-      <c r="M5">
+      <c r="M6">
         <v>5</v>
       </c>
-      <c r="N5">
+      <c r="N6">
         <v>3</v>
       </c>
-      <c r="O5">
+      <c r="O6">
         <v>4</v>
       </c>
     </row>

</xml_diff>